<commit_message>
version 1.3 - Matching with TGF
</commit_message>
<xml_diff>
--- a/external/Mismatch sheet.xlsx
+++ b/external/Mismatch sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d4a9fd65a6bad53/Seun/2. Career and business/3. IQVIA-Asiwaju-PC/Analysis/tHFA/external/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{A38DAB68-A8AA-49F9-A005-451030428CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{535B86D5-95AA-432A-BC15-FACB05E873B6}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{A38DAB68-A8AA-49F9-A005-451030428CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC9C50D3-26F6-4004-9ACB-E5177B828961}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{D183F698-2D91-4878-B225-9023F2354C75}"/>
   </bookViews>
@@ -37,8 +37,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0663422C-2517-4800-A87D-7EC10347B720}</author>
+  </authors>
+  <commentList>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{0663422C-2517-4800-A87D-7EC10347B720}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Treat DNK as NO</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="78">
   <si>
     <t>KPI</t>
   </si>
@@ -190,9 +208,6 @@
     <t>Examples</t>
   </si>
   <si>
-    <t>MWI_000491</t>
-  </si>
-  <si>
     <t>NaN (Pan) - 0 (Seun)</t>
   </si>
   <si>
@@ -232,9 +247,6 @@
     <t>MWI_000019</t>
   </si>
   <si>
-    <t>Pankhuri/Seun</t>
-  </si>
-  <si>
     <t>"DNK" should nullify the entire attribute</t>
   </si>
   <si>
@@ -242,13 +254,50 @@
   </si>
   <si>
     <t>Larger discussion about that</t>
+  </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>Different ways of treating "Reported, Not seen"</t>
+  </si>
+  <si>
+    <t>Discuss with Emeka &amp; Pankhuri</t>
+  </si>
+  <si>
+    <t>MWI_000007</t>
+  </si>
+  <si>
+    <t>Seun - averaged response scores across the indicator without client first</t>
+  </si>
+  <si>
+    <t>MWI_001038, MWI_000877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seun </t>
+  </si>
+  <si>
+    <t>Pankhuri - Averaged dossiers first for disease then for dimension
+Code on ANC calc.</t>
+  </si>
+  <si>
+    <t>0 (Pan) - NaN (Seun)</t>
+  </si>
+  <si>
+    <t>MWI_000436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failed </t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +313,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -273,7 +334,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -305,11 +366,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -320,6 +392,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,6 +412,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Seun Osonuga" id="{A960B693-31F7-4E0A-9F07-34E3AA609119}" userId="6d4a9fd65a6bad53" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -632,12 +715,21 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E15" dT="2024-08-09T08:45:01.62" personId="{A960B693-31F7-4E0A-9F07-34E3AA609119}" id="{0663422C-2517-4800-A87D-7EC10347B720}">
+    <text>Treat DNK as NO</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B41FD8-E45E-4BB4-BA2E-D44707CFAA12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B41FD8-E45E-4BB4-BA2E-D44707CFAA12}">
+  <sheetPr filterMode="1"/>
   <dimension ref="B2:K36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -646,7 +738,7 @@
     <col min="2" max="2" width="25.26953125" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="14.36328125" customWidth="1"/>
-    <col min="5" max="5" width="22.08984375" customWidth="1"/>
+    <col min="5" max="5" width="31.81640625" customWidth="1"/>
     <col min="6" max="6" width="15.36328125" customWidth="1"/>
     <col min="7" max="7" width="13.1796875" customWidth="1"/>
     <col min="8" max="8" width="14.54296875" customWidth="1"/>
@@ -680,7 +772,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -688,12 +780,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
@@ -704,13 +800,24 @@
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
@@ -720,21 +827,22 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
@@ -744,17 +852,22 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
@@ -764,20 +877,23 @@
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
@@ -788,13 +904,16 @@
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
+      <c r="J8" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
@@ -804,15 +923,18 @@
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="J9" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -820,7 +942,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -828,7 +950,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -836,7 +958,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -844,7 +966,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
@@ -852,7 +974,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -860,7 +982,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
@@ -868,7 +990,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -884,18 +1006,21 @@
         <v>20</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.35">
@@ -906,21 +1031,23 @@
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="H15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
@@ -930,7 +1057,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -946,21 +1073,25 @@
         <v>23</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
@@ -968,7 +1099,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -976,7 +1107,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
@@ -984,7 +1115,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -992,7 +1123,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1000,7 +1131,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1008,7 +1139,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1016,7 +1147,7 @@
         <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1024,7 +1155,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1032,7 +1163,7 @@
         <v>29</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1040,7 +1171,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
@@ -1048,7 +1179,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1056,7 +1187,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
@@ -1064,7 +1195,7 @@
         <v>31</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1072,21 +1203,23 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1094,7 +1227,7 @@
         <v>33</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -1102,7 +1235,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1110,15 +1243,21 @@
         <v>35</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>34</v>
       </c>
@@ -1126,15 +1265,19 @@
         <v>36</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1142,15 +1285,19 @@
         <v>37</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1158,15 +1305,19 @@
         <v>38</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1174,15 +1325,19 @@
         <v>39</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
         <v>34</v>
       </c>
@@ -1190,15 +1345,19 @@
         <v>40</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
         <v>41</v>
       </c>
@@ -1206,21 +1365,24 @@
         <v>42</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
         <v>41</v>
       </c>
@@ -1228,19 +1390,22 @@
         <v>43</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>44</v>
       </c>
@@ -1248,25 +1413,28 @@
         <v>44</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="G35" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>45</v>
       </c>
@@ -1274,7 +1442,7 @@
         <v>45</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1283,7 +1451,17 @@
       <c r="I36" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:I36" xr:uid="{E8B41FD8-E45E-4BB4-BA2E-D44707CFAA12}"/>
+  <autoFilter ref="B2:I36" xr:uid="{E8B41FD8-E45E-4BB4-BA2E-D44707CFAA12}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="KPI S1 - Integrated services"/>
+        <filter val="KPI S2 - ISS"/>
+        <filter val="KPI S5 - System CHWs"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>